<commit_message>
bardziej odjebane wykresy - wersja finalna
</commit_message>
<xml_diff>
--- a/Alternatywne_I/Dane.xlsx
+++ b/Alternatywne_I/Dane.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27960" windowHeight="13875"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27960" windowHeight="13875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zacienienie" sheetId="1" r:id="rId1"/>
@@ -105,18 +105,6 @@
   </si>
   <si>
     <t>_25</t>
-  </si>
-  <si>
-    <t>Filename	     Date &amp; Time	Tc</t>
-  </si>
-  <si>
-    <t>[degC]	 Is</t>
-  </si>
-  <si>
-    <t>c [mA]	 Voc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[mV]	</t>
   </si>
   <si>
     <t xml:space="preserve">Im [mA]	</t>
@@ -358,23 +346,28 @@
       <t>C</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Voc [mV]	</t>
+  </si>
+  <si>
+    <t>Isc [mA]</t>
+  </si>
+  <si>
+    <t>Tc [degC]</t>
+  </si>
+  <si>
+    <t>Filename	     Date &amp; Tim</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Czcionka tekstu podstawowego"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,9 +412,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -435,6 +428,38 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Wpływ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> zacienienia na wydajność ogniwa</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -5001,8 +5026,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.8803735706302127E-2"/>
-                  <c:y val="3.5833356239062517E-2"/>
+                  <c:x val="-3.8803735706302148E-2"/>
+                  <c:y val="3.583335623906253E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -5126,7 +5151,7 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.4388810076519544E-2"/>
+                  <c:x val="-9.438881007651953E-2"/>
                   <c:y val="2.5599442932666319E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -5166,8 +5191,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.12678198349239103"/>
-                  <c:y val="-2.0944998763090625E-2"/>
+                  <c:x val="-0.12678198349239114"/>
+                  <c:y val="-2.0944998763090632E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -5314,8 +5339,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.12283993207806713"/>
-                  <c:y val="4.8871663780544791E-2"/>
+                  <c:x val="-0.12283993207806711"/>
+                  <c:y val="4.8871663780544777E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -5387,14 +5412,14 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="62423808"/>
-        <c:axId val="62425344"/>
+        <c:axId val="118230016"/>
+        <c:axId val="118252672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62423808"/>
+        <c:axId val="118230016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.70000000000000007"/>
+          <c:max val="0.70000000000000029"/>
           <c:min val="-0.5"/>
         </c:scaling>
         <c:axPos val="b"/>
@@ -5406,10 +5431,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>U [V]</a:t>
                 </a:r>
               </a:p>
@@ -5422,12 +5447,12 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="62425344"/>
+        <c:crossAx val="118252672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62425344"/>
+        <c:axId val="118252672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -5442,14 +5467,14 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>I</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
                   <a:t> [A]</a:t>
                 </a:r>
               </a:p>
@@ -5462,7 +5487,7 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="62423808"/>
+        <c:crossAx val="118230016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5470,12 +5495,25 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5485,6 +5523,38 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Wpływ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> temperatury na wydajność ogniwa</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -10323,8 +10393,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.9946909122173503E-2"/>
-                  <c:y val="-3.891663493099759E-2"/>
+                  <c:x val="-3.9946909122173517E-2"/>
+                  <c:y val="-3.8916634930997576E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -10368,7 +10438,7 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2676683002321379E-2"/>
+                  <c:x val="-4.2676683002321407E-2"/>
                   <c:y val="3.4782474656801406E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -10489,8 +10559,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.1275555627203164"/>
-                  <c:y val="-1.612171989191738E-2"/>
+                  <c:x val="-0.12755556272031637"/>
+                  <c:y val="-1.6121719891917387E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -10530,8 +10600,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2862823488951938E-3"/>
-                  <c:y val="2.7637234100429793E-2"/>
+                  <c:x val="-4.2862823488951964E-3"/>
+                  <c:y val="2.7637234100429814E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -10652,7 +10722,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.12972562548362135"/>
-                  <c:y val="2.0727925575322343E-2"/>
+                  <c:y val="2.0727925575322353E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -10684,7 +10754,7 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.0971434098529793E-2"/>
+                  <c:x val="-2.0971434098529796E-2"/>
                   <c:y val="-3.454654262553724E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -10763,14 +10833,14 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="120937088"/>
-        <c:axId val="153371008"/>
+        <c:axId val="120015104"/>
+        <c:axId val="119868800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120937088"/>
+        <c:axId val="120015104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.70000000000000007"/>
+          <c:max val="0.70000000000000029"/>
           <c:min val="-0.5"/>
         </c:scaling>
         <c:axPos val="b"/>
@@ -10782,17 +10852,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>U</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
                   <a:t> [V]</a:t>
                 </a:r>
-                <a:endParaRPr lang="pl-PL"/>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -10803,12 +10873,12 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="153371008"/>
+        <c:crossAx val="119868800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153371008"/>
+        <c:axId val="119868800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -10823,10 +10893,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1200"/>
                   <a:t>I [A]</a:t>
                 </a:r>
               </a:p>
@@ -10839,7 +10909,7 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="120937088"/>
+        <c:crossAx val="120015104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10847,12 +10917,935 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wpływ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> temperatury ogniwa na jesgo sprawność</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Temperatura!$D$2,Temperatura!$D$4,Temperatura!$D$6,Temperatura!$D$8,Temperatura!$D$10:$D$43)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>21.7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Temperatura!$K$2,Temperatura!$K$4,Temperatura!$K$6,Temperatura!$K$8,Temperatura!$K$10:$K$43)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.06</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.05</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.93</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.88</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.79</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.69</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.61</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.53</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12.67</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.71</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.88</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.94</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.14</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.28</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.34</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.42</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.54</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.79</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13.72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13.72</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13.92</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14.15</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14.08</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14.11</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Temperatura!$D$3,Temperatura!$D$5,Temperatura!$D$7,Temperatura!$D$9)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Temperatura!$K$3,Temperatura!$K$5,Temperatura!$K$7,Temperatura!$K$9)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="119908992"/>
+        <c:axId val="120104448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="119908992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="55"/>
+          <c:min val="15"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>T [°C]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050"/>
+        </c:spPr>
+        <c:crossAx val="120104448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120104448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="14.5"/>
+          <c:min val="11"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1200" b="1"/>
+                  <a:t>η</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" b="1"/>
+                  <a:t> [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050"/>
+        </c:spPr>
+        <c:crossAx val="119908992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wpływ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> temperatury ogniwa na napięcie U</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="-25000"/>
+              <a:t>OC</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Temperatura!$D$2:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>46.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>52.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>52.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>48.1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30.9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>21.7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Temperatura!$F$2:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>614.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>614.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>612.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>608.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>624.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>616.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>615.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>613.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>615.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>604</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>602.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>599.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>604.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>598.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>595.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>593.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>589.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>587.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>583.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>580.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>573.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>574.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>565.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>565.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>563.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>570.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>580.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>583.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>587.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>589.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>595.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>597.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>597.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>608.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>607.1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>617.1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>623.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>628.1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>626.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>629.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>630</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="120193024"/>
+        <c:axId val="120196096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="120193024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="55"/>
+          <c:min val="15"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>T</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t> [°C]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050"/>
+        </c:spPr>
+        <c:crossAx val="120196096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120196096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>U</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="-25000"/>
+                  <a:t>OC </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t>[mV]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050"/>
+        </c:spPr>
+        <c:crossAx val="120193024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10869,9 +11862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>684674</xdr:colOff>
+      <xdr:colOff>379874</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>170773</xdr:rowOff>
+      <xdr:rowOff>113623</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10899,9 +11892,74 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>618000</xdr:colOff>
+      <xdr:colOff>313200</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>151725</xdr:rowOff>
+      <xdr:rowOff>37425</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Wykres 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>522749</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>46950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>532275</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>132675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11230,8 +12288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF66" sqref="AF66"/>
+    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11284,7 +12342,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>26.9</v>
@@ -11296,13 +12354,13 @@
         <v>52.3</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q3">
         <v>19.5</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -11324,37 +12382,37 @@
         <v>1060.9000000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G5">
         <v>1059.7</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L5">
         <v>1036.3</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Q5">
         <v>1046.0999999999999</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -13505,7 +14563,7 @@
     </row>
     <row r="43" spans="1:20" ht="18.75">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B43">
         <v>-1.22327E-3</v>
@@ -13522,7 +14580,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G43">
         <v>2.4465300000000001E-3</v>
@@ -13553,7 +14611,7 @@
         <v>0</v>
       </c>
       <c r="P43" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q43">
         <v>3.6698E-3</v>
@@ -13600,7 +14658,7 @@
         <v>0</v>
       </c>
       <c r="K44" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L44">
         <v>6.1163000000000005E-4</v>
@@ -24203,7 +25261,7 @@
         <v>0</v>
       </c>
       <c r="F227" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G227">
         <v>0.61469165999999997</v>
@@ -25294,7 +26352,7 @@
     </row>
     <row r="246" spans="1:20" ht="18.75">
       <c r="A246" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B246">
         <v>0.6153033</v>
@@ -25325,7 +26383,7 @@
         <v>0</v>
       </c>
       <c r="K246" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L246">
         <v>0.56514934999999999</v>
@@ -25632,7 +26690,7 @@
         <v>0</v>
       </c>
       <c r="P251" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Q251">
         <v>0.62692433000000003</v>
@@ -33369,8 +34427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -33393,42 +34451,42 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
         <f>TIMEVALUE(MID(B2,19,5))</f>
@@ -33467,10 +34525,10 @@
     </row>
     <row r="3" spans="1:13">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C19" si="0">TIMEVALUE(MID(B3,19,5))</f>
+        <f t="shared" ref="C3:C15" si="0">TIMEVALUE(MID(B3,19,5))</f>
         <v>0.52222222222222225</v>
       </c>
       <c r="D3" s="1">
@@ -33506,7 +34564,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
@@ -33545,7 +34603,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
@@ -33584,7 +34642,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
@@ -33623,7 +34681,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="B7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
@@ -33662,7 +34720,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="B8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
@@ -33701,7 +34759,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
@@ -33743,7 +34801,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
@@ -33782,7 +34840,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
@@ -33821,7 +34879,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
@@ -33860,7 +34918,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
@@ -33899,7 +34957,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="B14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
@@ -33938,7 +34996,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
@@ -33977,7 +35035,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="B16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2">
         <f>TIMEVALUE(MID(B16,20,5))</f>
@@ -34016,10 +35074,10 @@
     </row>
     <row r="17" spans="1:13">
       <c r="B17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" ref="C17:C20" si="1">TIMEVALUE(MID(B17,20,5))</f>
+        <f t="shared" ref="C17:C19" si="1">TIMEVALUE(MID(B17,20,5))</f>
         <v>0.54027777777777775</v>
       </c>
       <c r="D17" s="1">
@@ -34055,7 +35113,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="B18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -34094,7 +35152,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
@@ -34133,7 +35191,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2">
         <f>TIMEVALUE(MID(B20,16,5))</f>
@@ -34172,10 +35230,10 @@
     </row>
     <row r="21" spans="1:13">
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:C28" si="2">TIMEVALUE(MID(B21,16,5))</f>
+        <f t="shared" ref="C21:C27" si="2">TIMEVALUE(MID(B21,16,5))</f>
         <v>0.54375000000000007</v>
       </c>
       <c r="D21" s="1">
@@ -34211,7 +35269,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="B22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="2"/>
@@ -34250,7 +35308,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="B23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="2"/>
@@ -34289,7 +35347,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="B24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="2"/>
@@ -34328,7 +35386,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="B25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="2"/>
@@ -34367,10 +35425,10 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="2"/>
@@ -34409,10 +35467,10 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="2"/>
@@ -34451,7 +35509,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2">
         <f>TIMEVALUE(MID(B28,17,5))</f>
@@ -34490,7 +35548,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="B29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" ref="C29:C43" si="3">TIMEVALUE(MID(B29,17,5))</f>
@@ -34529,7 +35587,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="B30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="3"/>
@@ -34568,7 +35626,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="B31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="3"/>
@@ -34607,7 +35665,7 @@
     </row>
     <row r="32" spans="1:13">
       <c r="B32" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="3"/>
@@ -34646,7 +35704,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="B33" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="3"/>
@@ -34685,7 +35743,7 @@
     </row>
     <row r="34" spans="1:13">
       <c r="B34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="3"/>
@@ -34724,7 +35782,7 @@
     </row>
     <row r="35" spans="1:13">
       <c r="B35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="3"/>
@@ -34763,7 +35821,7 @@
     </row>
     <row r="36" spans="1:13">
       <c r="B36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" si="3"/>
@@ -34802,7 +35860,7 @@
     </row>
     <row r="37" spans="1:13">
       <c r="B37" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="3"/>
@@ -34841,7 +35899,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="B38" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" si="3"/>
@@ -34880,7 +35938,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="B39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" si="3"/>
@@ -34919,7 +35977,7 @@
     </row>
     <row r="40" spans="1:13">
       <c r="B40" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="3"/>
@@ -34958,7 +36016,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="B41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="3"/>
@@ -34997,7 +36055,7 @@
     </row>
     <row r="42" spans="1:13">
       <c r="B42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" si="3"/>
@@ -35036,10 +36094,10 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" t="s">
         <v>62</v>
-      </c>
-      <c r="B43" t="s">
-        <v>66</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="3"/>
@@ -35049,10 +36107,10 @@
         <v>19.5</v>
       </c>
       <c r="E43" s="1">
-        <v>27.9</v>
+        <v>8027.9</v>
       </c>
       <c r="F43" s="1">
-        <v>30</v>
+        <v>630</v>
       </c>
       <c r="G43" s="1">
         <v>7410.1</v>
@@ -35078,11 +36136,12 @@
     </row>
     <row r="46" spans="1:13">
       <c r="M46" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>